<commit_message>
Update demand by node description in table definitions
</commit_message>
<xml_diff>
--- a/data/example/Power_Demand_KInRows.xlsx
+++ b/data/example/Power_Demand_KInRows.xlsx
@@ -811,7 +811,7 @@
       </c>
       <c r="G5" s="8" t="inlineStr">
         <is>
-          <t>Demand at node for representative node i</t>
+          <t>Demand at node at node i</t>
         </is>
       </c>
       <c r="H5" s="7" t="n"/>
@@ -18685,7 +18685,7 @@
       </c>
       <c r="G5" s="8" t="inlineStr">
         <is>
-          <t>Demand at node for representative node i</t>
+          <t>Demand at node at node i</t>
         </is>
       </c>
       <c r="H5" s="7" t="n"/>

</xml_diff>